<commit_message>
Adding additional performance tests
</commit_message>
<xml_diff>
--- a/ml_files/combined_test_results.xlsx
+++ b/ml_files/combined_test_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Test</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">MCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUPR</t>
   </si>
   <si>
     <t xml:space="preserve">error</t>
@@ -230,10 +233,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -298,13 +301,16 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0.81</v>
@@ -371,7 +377,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.9</v>
@@ -438,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.56</v>
@@ -505,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0.95</v>
@@ -572,7 +578,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0.94</v>
@@ -639,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0.94</v>
@@ -706,7 +712,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0.8</v>
@@ -773,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0.94</v>
@@ -840,7 +846,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0.94</v>
@@ -907,7 +913,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0.93</v>
@@ -974,7 +980,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0.61</v>
@@ -1041,7 +1047,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0.94</v>
@@ -1108,7 +1114,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0.94</v>
@@ -1175,7 +1181,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0.94</v>
@@ -1242,7 +1248,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0.9</v>
@@ -1309,7 +1315,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0.93</v>
@@ -1376,7 +1382,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0.93</v>
@@ -1443,7 +1449,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0.93</v>

</xml_diff>